<commit_message>
base dao service 课堂跟进练习  2019-4-15 22:55:46
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,30 @@
   </si>
   <si>
     <t>21:00--21:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年4月15日22:54:03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课堂跟进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:30--10:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base dao service课后练习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:30--18:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -700,6 +724,28 @@
         <v>42</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
base dao service课后练习（已整合至My_Sun工程）测试已完成  2019-4-16 13:11:35
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,22 @@
   </si>
   <si>
     <t>16:30--18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年4月16日13:09:33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:00--13:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base dao service课后练习（已整合至My_Sun工程）测试已完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -540,16 +556,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="43.75" customWidth="1"/>
+    <col min="3" max="3" width="60.875" customWidth="1"/>
     <col min="4" max="4" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -746,6 +762,20 @@
         <v>48</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
star项目构建 Hibernate跟进学习  2019-4-24 23:05:21
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -270,6 +270,38 @@
   </si>
   <si>
     <t>22:00--23:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年4月24日23:01:24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hibernate练习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:30--10:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star项目构建（base，dao）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star项目构建（base，dao）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:00--15:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:00--24:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -854,6 +886,36 @@
         <v>62</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
star -- base and dao -- Entity and Test  2019-4-25 23:26:56
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,6 +302,30 @@
   </si>
   <si>
     <t>23:00--24:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年4月25日23:23:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>业务实体domain Entity ER建模</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30--12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:30--21:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star项目构建（base，dao）Entity and Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -916,6 +940,28 @@
         <v>70</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DaoTest 空指针异常  2019-4-25 23:49:47
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -326,6 +326,14 @@
   </si>
   <si>
     <t>star项目构建（base，dao）Entity and Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoleDaoTest 空指针异常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23:30--23:45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -652,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -962,6 +970,14 @@
         <v>75</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dao service  2019-5-8 23:53:29
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -470,6 +470,30 @@
   </si>
   <si>
     <t>事物回滚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月8日23:51:54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dao service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:00--16:40 &amp; 19:00--21:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dao service bug修正，未完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22:40--23:50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -796,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1236,6 +1260,28 @@
         <v>111</v>
       </c>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dao service 完善  2019-5-9 23:10:45
</commit_message>
<xml_diff>
--- a/201708044226Ly/201708044226Ly.xlsx
+++ b/201708044226Ly/201708044226Ly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
   <si>
     <t>周一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -494,6 +494,34 @@
   </si>
   <si>
     <t>22:40--23:50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019年5月9日23:05:28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dao service bug修正，完善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JavaEE上机完善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互控制 Controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:30--12:00 &amp; 13:30--15:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:30--19:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -820,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1282,6 +1310,36 @@
         <v>118</v>
       </c>
     </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>